<commit_message>
UPDATE: tache liaison BDD terminé et correction d'un bug
</commit_message>
<xml_diff>
--- a/docs/Diagramme de Gantt.xlsx
+++ b/docs/Diagramme de Gantt.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3101968-DFF2-4E00-AB58-3B6DE42B456D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DA73BE-01B7-4635-8DEC-EE8FD21AD21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5868" yWindow="48" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PlanningProjet" sheetId="11" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="90">
   <si>
     <t>Créez un planning de projet dans cette feuille de calcul.
 Entrez le titre de ce projet dans la cellule B1. 
@@ -342,10 +342,13 @@
     <t>22H</t>
   </si>
   <si>
-    <t>0H15</t>
-  </si>
-  <si>
-    <t>76H50</t>
+    <t>1H20</t>
+  </si>
+  <si>
+    <t>2H20</t>
+  </si>
+  <si>
+    <t>77H55</t>
   </si>
 </sst>
 </file>
@@ -2119,8 +2122,8 @@
   <dimension ref="A1:CG47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <pane ySplit="7" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2189,7 +2192,7 @@
         <v>75</v>
       </c>
       <c r="E4" s="94" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F4" s="95"/>
     </row>
@@ -3478,7 +3481,7 @@
       <c r="E13" s="98"/>
       <c r="F13" s="98"/>
       <c r="G13" s="98" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="H13" s="13"/>
       <c r="I13" s="30"/>
@@ -3568,15 +3571,15 @@
         <v>43</v>
       </c>
       <c r="D14" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="100">
-        <f>DATE(14,1,14)</f>
-        <v>5128</v>
+        <f>DATE(2023,1,14)</f>
+        <v>44940</v>
       </c>
       <c r="F14" s="100">
         <f>E14</f>
-        <v>5128</v>
+        <v>44940</v>
       </c>
       <c r="G14" s="100" t="s">
         <v>87</v>
@@ -3673,11 +3676,11 @@
       </c>
       <c r="E15" s="100">
         <f>E14</f>
-        <v>5128</v>
+        <v>44940</v>
       </c>
       <c r="F15" s="100">
         <f>E15</f>
-        <v>5128</v>
+        <v>44940</v>
       </c>
       <c r="G15" s="100" t="s">
         <v>59</v>
@@ -6905,12 +6908,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7202,29 +7216,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7251,13 +7258,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>